<commit_message>
changes and Projects for econ 470
</commit_message>
<xml_diff>
--- a/jdocs/Stats/FinalGradeCheck.xlsx
+++ b/jdocs/Stats/FinalGradeCheck.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="22035" windowHeight="10035"/>
+    <workbookView xWindow="120" yWindow="36" windowWidth="19296" windowHeight="10032"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -274,6 +274,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -482,7 +550,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="F0F0F0"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -764,14 +832,14 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -782,7 +850,7 @@
       <c r="C1" s="18"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16" t="s">
         <v>2</v>
@@ -794,96 +862,96 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3">
         <f>B3*C3</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D7" si="0">B4*C4</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>230</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>230</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>230</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1">
-        <v>330</v>
+        <v>33</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>330</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="5">
         <f>SUM(B3:B7)</f>
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5">
         <f>SUM(D3:D7)</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -907,7 +975,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>4</v>
       </c>
@@ -945,7 +1013,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -957,7 +1025,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>